<commit_message>
working code for assert implemented fucntionality
</commit_message>
<xml_diff>
--- a/testData/abcs.xlsx
+++ b/testData/abcs.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://talentkloud-my.sharepoint.com/personal/vaibhav_gangrade_codvo_ai/Documents/Documents/Codvo.ai/MyProject/ZS_GenAI/testData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://talentkloud-my.sharepoint.com/personal/vaibhav_gangrade_codvo_ai/Documents/Documents/Codvo.ai/MyProject/ZS_Playwright_GenAI/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="183" documentId="13_ncr:1_{054CADDF-AA3E-4041-98F7-EE3BCD8AE219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E55B642-B3AD-4F17-9A9E-2F53D0EF31AD}"/>
+  <xr:revisionPtr revIDLastSave="206" documentId="13_ncr:1_{054CADDF-AA3E-4041-98F7-EE3BCD8AE219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51B7EB19-A4AE-4C98-A93A-9A53D0E2C222}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>action</t>
   </si>
@@ -48,55 +49,49 @@
     <t>https://www.amazon.com/</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>click</t>
   </si>
   <si>
     <t>Hello, Sign in</t>
   </si>
   <si>
-    <t>email input field</t>
-  </si>
-  <si>
-    <t>weavernormar@gmail.com</t>
-  </si>
-  <si>
-    <t>Continue button on page</t>
-  </si>
-  <si>
-    <t>password input field in span</t>
-  </si>
-  <si>
-    <t>Welcome@123456</t>
-  </si>
-  <si>
-    <t>signin button on page</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/gp/cart/view.html?ref_=nav_cart</t>
-  </si>
-  <si>
-    <t>assert</t>
-  </si>
-  <si>
-    <t>h2#deliver-to-customer-text</t>
-  </si>
-  <si>
-    <t>Delivering to Normar Weaver</t>
-  </si>
-  <si>
     <t>waitfortext</t>
   </si>
   <si>
-    <t>Continue</t>
-  </si>
-  <si>
-    <t>checkvisible</t>
-  </si>
-  <si>
-    <t>Proceed to checkout</t>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>https://www.bluenile.com/jewelry/necklaces/lab-grown-diamond-cushion-cut-solitaire-pendant-in-14k-white-gold-1-2-ct-tw-f-g-vs2-si1-item-202314</t>
+  </si>
+  <si>
+    <t>scroll</t>
+  </si>
+  <si>
+    <t>Ships by</t>
+  </si>
+  <si>
+    <t>ADD TO CART button</t>
+  </si>
+  <si>
+    <t>TID</t>
+  </si>
+  <si>
+    <t>Execution</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>clickto</t>
+  </si>
+  <si>
+    <t>ai_click</t>
   </si>
 </sst>
 </file>
@@ -433,7 +428,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,18 +471,18 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="E4" s="1">
         <v>3000</v>
@@ -495,119 +490,99 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E5" s="1">
+        <v>9000</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1000</v>
       </c>
       <c r="E6" s="1">
-        <v>2000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1000</v>
       </c>
       <c r="E7" s="1">
-        <v>3000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="1">
-        <v>3000</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="1">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="1">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="1">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="B10" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1" xr:uid="{BA0E224C-C858-47AF-8859-A659DB8B5C6D}"/>
-    <hyperlink ref="C8" r:id="rId2" xr:uid="{AB3D6231-B488-4B94-BF6C-F9D8D7D5C450}"/>
-    <hyperlink ref="B10" r:id="rId3" xr:uid="{7C565A3A-1F61-43E8-B522-18E058CC5652}"/>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{8E714C0B-2E42-402D-AB9A-5C765378CBA1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F87356D-01B6-4AE7-B5F6-76DEA25ED588}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>